<commit_message>
Added sheet for 7th April
</commit_message>
<xml_diff>
--- a/Daily Status update Report 01042020.xlsx
+++ b/Daily Status update Report 01042020.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="31-Mar" sheetId="9" r:id="rId9"/>
     <sheet name="01-Apr" sheetId="11" r:id="rId10"/>
     <sheet name="03-Apr" sheetId="12" r:id="rId11"/>
+    <sheet name="07-Apr" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="116">
   <si>
     <t>Employee Name</t>
   </si>
@@ -382,8 +383,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -819,21 +820,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -844,7 +845,7 @@
     <col min="7" max="7" width="117.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -867,7 +868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -890,7 +891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -913,7 +914,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -936,7 +937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -959,7 +960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -982,7 +983,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1051,7 +1052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1074,7 +1075,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1118,7 +1119,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1146,14 +1147,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1164,7 +1165,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1187,7 +1188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1233,7 +1234,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1302,7 +1303,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1325,7 +1326,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1348,7 +1349,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1371,7 +1372,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1417,7 +1418,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1493,12 +1494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1509,7 +1512,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1553,7 +1556,7 @@
       </c>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1574,7 +1577,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1595,7 +1598,7 @@
       </c>
       <c r="G4" s="31"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1616,7 +1619,7 @@
       </c>
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1637,7 +1640,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1658,7 +1661,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1679,7 +1682,7 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1700,7 +1703,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1721,7 +1724,7 @@
       </c>
       <c r="G10" s="32"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1742,7 +1745,7 @@
       </c>
       <c r="G11" s="32"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1763,7 +1766,7 @@
       </c>
       <c r="G12" s="32"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1784,7 +1787,327 @@
       </c>
       <c r="G13" s="32"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
+      <c r="A14" s="33">
+        <v>13</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="34">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G14" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="29">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F2" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="29">
+        <v>0.40625</v>
+      </c>
+      <c r="F3" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.40625</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G4" s="31"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="29">
+        <v>0.40625</v>
+      </c>
+      <c r="F5" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="29">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F6" s="29">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F7" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F8" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="29">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="32">
+        <v>9</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="30">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F10" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="32">
+        <v>10</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="30">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="32"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="32">
+        <v>11</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="30">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="32">
+        <v>12</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="30">
+        <v>0.375</v>
+      </c>
+      <c r="F13" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1811,14 +2134,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1829,7 +2152,7 @@
     <col min="7" max="7" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1852,7 +2175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1875,7 +2198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1898,7 +2221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1921,7 +2244,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1944,7 +2267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1967,7 +2290,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1990,7 +2313,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2013,7 +2336,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2036,7 +2359,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2059,7 +2382,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2082,7 +2405,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2105,7 +2428,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2135,14 +2458,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2153,7 +2476,7 @@
     <col min="7" max="7" width="136.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2176,7 +2499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2199,7 +2522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2222,7 +2545,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2245,7 +2568,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2268,7 +2591,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2291,7 +2614,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2314,7 +2637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2337,7 +2660,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2360,7 +2683,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2383,7 +2706,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2406,7 +2729,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2429,7 +2752,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2459,14 +2782,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2477,7 +2800,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2500,7 +2823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2523,7 +2846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2546,7 +2869,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2569,7 +2892,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2592,7 +2915,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2615,7 +2938,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2638,7 +2961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2661,7 +2984,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2684,7 +3007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2707,7 +3030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2730,7 +3053,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2753,7 +3076,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2776,7 +3099,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2806,14 +3129,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -2824,7 +3147,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2847,7 +3170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2870,7 +3193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2893,7 +3216,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2916,7 +3239,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2939,7 +3262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2962,7 +3285,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2985,7 +3308,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3008,7 +3331,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3031,7 +3354,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3054,7 +3377,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3077,7 +3400,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3100,7 +3423,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3123,7 +3446,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3153,14 +3476,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3171,7 +3494,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3194,7 +3517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3217,7 +3540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3240,7 +3563,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3263,7 +3586,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3286,7 +3609,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3309,7 +3632,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3332,7 +3655,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3355,7 +3678,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3378,7 +3701,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3401,7 +3724,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3424,7 +3747,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3447,7 +3770,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3470,7 +3793,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3500,14 +3823,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3518,7 +3841,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3541,7 +3864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3564,7 +3887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3587,7 +3910,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3610,7 +3933,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3633,7 +3956,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3656,7 +3979,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3679,7 +4002,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3702,7 +4025,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3725,7 +4048,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3748,7 +4071,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3771,7 +4094,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3794,7 +4117,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3817,7 +4140,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3847,14 +4170,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -3865,7 +4188,7 @@
     <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
@@ -3888,7 +4211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3911,7 +4234,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -3934,7 +4257,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -3957,7 +4280,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -3980,7 +4303,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -4003,7 +4326,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -4026,7 +4349,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -4049,7 +4372,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -4072,7 +4395,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -4095,7 +4418,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -4118,7 +4441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -4141,7 +4464,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -4164,7 +4487,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -4194,14 +4517,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -4212,7 +4535,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4235,7 +4558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4258,7 +4581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4281,7 +4604,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4304,7 +4627,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4327,7 +4650,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4350,7 +4673,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4373,7 +4696,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4396,7 +4719,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4419,7 +4742,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -4442,7 +4765,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -4465,7 +4788,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -4488,7 +4811,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -4511,7 +4834,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Status Updated for 3rd April
</commit_message>
<xml_diff>
--- a/Daily Status update Report 01042020.xlsx
+++ b/Daily Status update Report 01042020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="03-Apr" sheetId="12" r:id="rId11"/>
     <sheet name="07-Apr" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="117">
   <si>
     <t>Employee Name</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Created test cases for API Testing - Collateral flow (Deposit Cash - Unchecked /checked and Unchecked/Unchecked - Settled; All scenarios for Deposit Cash:Margin Deposit completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Git Basic Understanding Complete ; </t>
   </si>
 </sst>
 </file>
@@ -820,7 +823,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1497,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1783,9 +1786,11 @@
         <v>0.375</v>
       </c>
       <c r="F13" s="34">
-        <v>0.75</v>
-      </c>
-      <c r="G13" s="32"/>
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="33">
@@ -1817,7 +1822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated for  st april
</commit_message>
<xml_diff>
--- a/Daily Status update Report 01042020.xlsx
+++ b/Daily Status update Report 01042020.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="118">
   <si>
     <t>Employee Name</t>
   </si>
@@ -381,13 +381,16 @@
   </si>
   <si>
     <t xml:space="preserve">Git Basic Understanding Complete ; </t>
+  </si>
+  <si>
+    <t>Completed with Test Cases Writing for Collateral Withdraw Cash - Checked-Checked-Margin Deposit Scenario(for Created-&gt;Accepted-&gt; Settled)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -550,6 +553,9 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,21 +829,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -848,7 +854,7 @@
     <col min="7" max="7" width="117.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -871,7 +877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -894,7 +900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -917,7 +923,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -940,7 +946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -963,7 +969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -986,7 +992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1122,7 +1128,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1150,14 +1156,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1168,7 +1174,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1191,7 +1197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1214,7 +1220,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1237,7 +1243,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1283,7 +1289,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1306,7 +1312,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1329,7 +1335,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1352,7 +1358,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1398,7 +1404,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1467,7 +1473,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1497,14 +1503,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1515,7 +1521,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1559,7 +1565,7 @@
       </c>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1580,7 +1586,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1601,7 +1607,7 @@
       </c>
       <c r="G4" s="31"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1622,7 +1628,7 @@
       </c>
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1643,7 +1649,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1664,7 +1670,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1685,7 +1691,7 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1706,7 +1712,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1727,7 +1733,7 @@
       </c>
       <c r="G10" s="32"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1748,7 +1754,7 @@
       </c>
       <c r="G11" s="32"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1769,7 +1775,7 @@
       </c>
       <c r="G12" s="32"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1792,7 +1798,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1819,14 +1825,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1837,7 +1843,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1881,7 +1887,7 @@
       </c>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1902,7 +1908,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1923,7 +1929,7 @@
       </c>
       <c r="G4" s="31"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1944,7 +1950,7 @@
       </c>
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1965,7 +1971,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1986,7 +1992,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2007,7 +2013,7 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2028,7 +2034,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -2049,7 +2055,7 @@
       </c>
       <c r="G10" s="32"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -2068,9 +2074,11 @@
       <c r="F11" s="34">
         <v>0.75</v>
       </c>
-      <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -2091,7 +2099,7 @@
       </c>
       <c r="G12" s="32"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -2112,7 +2120,7 @@
       </c>
       <c r="G13" s="32"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -2139,14 +2147,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2157,7 +2165,7 @@
     <col min="7" max="7" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2180,7 +2188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2203,7 +2211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2226,7 +2234,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2249,7 +2257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2272,7 +2280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2295,7 +2303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2318,7 +2326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2341,7 +2349,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2364,7 +2372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2387,7 +2395,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2410,7 +2418,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2433,7 +2441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2463,14 +2471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2481,7 +2489,7 @@
     <col min="7" max="7" width="136.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2504,7 +2512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2527,7 +2535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2550,7 +2558,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2573,7 +2581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2596,7 +2604,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2619,7 +2627,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2642,7 +2650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2665,7 +2673,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2688,7 +2696,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2711,7 +2719,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2734,7 +2742,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2757,7 +2765,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2787,14 +2795,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2805,7 +2813,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2828,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2851,7 +2859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2874,7 +2882,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2897,7 +2905,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2920,7 +2928,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2943,7 +2951,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2966,7 +2974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2989,7 +2997,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3012,7 +3020,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3035,7 +3043,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3058,7 +3066,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3081,7 +3089,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3104,7 +3112,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3134,14 +3142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3152,7 +3160,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3175,7 +3183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3198,7 +3206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3221,7 +3229,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3244,7 +3252,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3267,7 +3275,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3290,7 +3298,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3313,7 +3321,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3336,7 +3344,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3359,7 +3367,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3382,7 +3390,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3405,7 +3413,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3428,7 +3436,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3451,7 +3459,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3481,14 +3489,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3499,7 +3507,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3522,7 +3530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3545,7 +3553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3568,7 +3576,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3591,7 +3599,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3614,7 +3622,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3637,7 +3645,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3660,7 +3668,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3683,7 +3691,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3706,7 +3714,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3729,7 +3737,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3752,7 +3760,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3775,7 +3783,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3798,7 +3806,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3828,14 +3836,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3846,7 +3854,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3869,7 +3877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3892,7 +3900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3915,7 +3923,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3938,7 +3946,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3961,7 +3969,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3984,7 +3992,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4007,7 +4015,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4030,7 +4038,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4053,7 +4061,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -4076,7 +4084,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -4099,7 +4107,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4122,7 +4130,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -4145,7 +4153,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -4175,14 +4183,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -4193,7 +4201,7 @@
     <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
@@ -4216,7 +4224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -4239,7 +4247,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -4262,7 +4270,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -4285,7 +4293,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -4308,7 +4316,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -4331,7 +4339,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -4354,7 +4362,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -4377,7 +4385,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -4400,7 +4408,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -4423,7 +4431,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -4446,7 +4454,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -4469,7 +4477,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -4492,7 +4500,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -4522,14 +4530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -4540,7 +4548,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4563,7 +4571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4586,7 +4594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4609,7 +4617,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4632,7 +4640,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4655,7 +4663,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4678,7 +4686,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4701,7 +4709,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4724,7 +4732,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4747,7 +4755,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -4770,7 +4778,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -4793,7 +4801,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -4816,7 +4824,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -4839,7 +4847,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
         <v>13</v>
       </c>

</xml_diff>